<commit_message>
updates excel file with addspecies output after checkign against last BLASTs and excel sheet with ADFG notes
</commit_message>
<xml_diff>
--- a/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies.xlsx
+++ b/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_A8619FD48F79A8D366075C52F37BD2725A413559" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8012B932-40EE-40F9-9BE6-C965FDACC924}"/>
+  <xr:revisionPtr revIDLastSave="376" documentId="11_A8619FD48F79A8D366075C52F37BD2725A413559" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A9D05CA-AA71-4611-BF56-1CF5D7CC961E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="388">
   <si>
     <t>rownames</t>
   </si>
@@ -1026,13 +1026,1276 @@
   </si>
   <si>
     <t>not in db!</t>
+  </si>
+  <si>
+    <t>100% match to database Myoxocephalus spp.</t>
+  </si>
+  <si>
+    <t>100% match to database Lepidopsetta spp.</t>
+  </si>
+  <si>
+    <t>100% match to gadidae;NA;NA</t>
+  </si>
+  <si>
+    <t>was in DB, but sequence in Db was longer; updated</t>
+  </si>
+  <si>
+    <t>was in DB, but sequence in Db was longer; did not match to Chesonia; updated</t>
+  </si>
+  <si>
+    <t>mutliple 100% matches: Chesnonia verrucosa, Occella dodecaedron &amp; Brachyopsis segaliensis</t>
+  </si>
+  <si>
+    <t>100% match to sebastes spp.</t>
+  </si>
+  <si>
+    <t>BLAST NOTES</t>
+  </si>
+  <si>
+    <t>99.37% eleginus gracilis, microgadus proximus</t>
+  </si>
+  <si>
+    <t>99.38% cluplea pallassii, 98.75% clupea harengus, Sprattus sprattus</t>
+  </si>
+  <si>
+    <t>99.36% Myoxocephalus scorpius, Myoxocephalus quadricornis, Myoxocephalis thompsonii, Megalocottus platycephalus, Myoxocephalus anaeus, Microcottus sellaris, Myoxocephalus stelleri, Myoxocephalus jaok, Myoxocephalus polyacanthocephalus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus stelleri</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus polyacanthocephalus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus jaok</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus quadricornis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microcottus sellaris</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus scorpius</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus thompsonii</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Megalocottus platycephalus</t>
+    </r>
+  </si>
+  <si>
+    <t>ADFG NOTES</t>
+  </si>
+  <si>
+    <t>DATABASE NOTES</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eleginus gracilis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microgadus proximus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spirinchus thaleichthys</t>
+    </r>
+  </si>
+  <si>
+    <t>Spirinchus thaleichthys</t>
+  </si>
+  <si>
+    <t>MATCHED NOTES</t>
+  </si>
+  <si>
+    <t>99.36% Osmerus mordax, 98.72% Sprinchus thaleichthys</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">100% matches: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus jaok</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myoxocephalus stelleri</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Myoxocephalus polyacanthocephalus </t>
+    </r>
+  </si>
+  <si>
+    <t>not found on ADFG notes sheet??</t>
+  </si>
+  <si>
+    <t>99.38% Clupea pallasii, Clupea harengus, 98.75% Sprattus sprattus</t>
+  </si>
+  <si>
+    <t>99.38% Clupea pallasii, 98.75% Clupea harengus, Sprattus sprattus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">100% matches: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lepidopsetta polyxystra (found in belugas)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lepidopsetta bilineata</t>
+    </r>
+  </si>
+  <si>
+    <t>99.38% Clupea palasii, 98.75% Clupea harengus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eleginus gracilis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microgadus proximus</t>
+    </r>
+  </si>
+  <si>
+    <t>GEOGRAPHIC NOTES</t>
+  </si>
+  <si>
+    <t>Sprattus sprattus is found in Europe</t>
+  </si>
+  <si>
+    <t>100% Sprattus sprattus, 99.38% clupea pallassii</t>
+  </si>
+  <si>
+    <t>100% Pungitus kaibarae, 99.36% Pungitus pungitus</t>
+  </si>
+  <si>
+    <t>Pungitus kaibarae not found in Alaska??</t>
+  </si>
+  <si>
+    <t>99.366% Osmerus mordax, 98.72% Spirinchus thaleichthys</t>
+  </si>
+  <si>
+    <t>99.37% Eleginus gracilis, 98.11% microgadus proximus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Eleginus gracilis, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microgadus proximus</t>
+    </r>
+  </si>
+  <si>
+    <t>microgaddus tomcod #1 match, but not found in Alaska</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% matches: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lumpenus sagitta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lumpenus fabricii</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Leptoclinus maculatus</t>
+    </r>
+  </si>
+  <si>
+    <t>Plausible by range, has been found in ice seal or beluga stomachs sorted by ADF&amp;G from the corresponding region- distinctions made based on if items have been found only in belugas or only in seal stomachs</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plausible by range, has </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>been found in ice seal or beluga stomachs sorted by ADF&amp;G from the corresponding region</t>
+    </r>
+  </si>
+  <si>
+    <t>Potentially plausible, species found just outside of documented range or is recognized as potentially in range in WORMS</t>
+  </si>
+  <si>
+    <t>Presence unlikely</t>
+  </si>
+  <si>
+    <t>Not plausible by range</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>NO MATCHES</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eleginus gracilis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microgadus proximus</t>
+    </r>
+  </si>
+  <si>
+    <t>not in db! Added</t>
+  </si>
+  <si>
+    <t>not in db! added</t>
+  </si>
+  <si>
+    <t>Podothecus accipenserinus</t>
+  </si>
+  <si>
+    <t>100% Sarritor frenatus, Leptagonus decagonus, Sarritor frenatus, Podothecus veternus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98%  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pleuronectes quadrituberculatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Platichthys stellatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hippoglossoides robustus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Liopsetta glacialis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hippoglossus stenolepis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reinhardtius hippoglossoides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Hippoglossoides elassodon, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myzopsetta proboscidea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parophrys vetulus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Glyptocephalus zachirus, Glyptocephalus stelleri, Isopsetta isolepis, Psettichthys melanostictus</t>
+    </r>
+  </si>
+  <si>
+    <t>99.36% Pungitus pungitus, Pungitus tymensis, Pungitus laevis</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parophrys vetulus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Glyptocephalus zachirus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reinhardtius hippoglossoides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pleuronectes quadrituberculatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myzopsetta proboscidea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Glyptocephalus stelleri</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Isopsetta isolepis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Psettichthys melanostictus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Platichthys stellatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hippoglossoides robustus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Liopsetta glacialis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hippoglossus stenolepis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hippoglossoides elassodon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no 100% matches: &gt;98% </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lepidopsetta bilineata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microstomus pacificus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lepidopsetta polyxystra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hippoglossoides robustus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Glyptocephalus zachirus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hippoglossoides elassodon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,  </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parophrys vetulus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Limanda sakhalinensis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pleuronectes quadrituberculatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Psettichthys melanostictus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Myzopsetta proboscidea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Platichthys stellatus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Liopsetta glacialis</t>
+    </r>
+  </si>
+  <si>
+    <t>99.366% Pungitus pungitus, Pungitus laevis</t>
+  </si>
+  <si>
+    <t>no 100% matches: &gt;98% Parophrys vetulus, Glyptocephalus zachirus, Reinhardtius hippoglossoides, Pleuronectes quadrituberculatus, Myzopsetta proboscidea, Glyptocephalus stelleri, Isopsetta isolepis, Psettichthys melanostictus, Platichthys stellatus, Hippoglossoides robustus, Liopsetta glacialis, Hippoglossus stenolepis, Hippoglossoides elassodon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1069,8 +2332,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1098,6 +2411,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1114,7 +2439,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1123,6 +2448,27 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1432,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I191"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5812,10 +7158,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7715EC1D-D232-4759-8D2A-5C5E9E00CDB6}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5827,10 +7173,14 @@
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="9" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="41.85546875" customWidth="1"/>
+    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5858,8 +7208,23 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -5881,11 +7246,12 @@
       <c r="G2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2"/>
+      <c r="K2" s="5" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -5904,11 +7270,17 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>343</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -5930,8 +7302,17 @@
       <c r="G4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>334</v>
+      </c>
+      <c r="L4" t="s">
+        <v>344</v>
+      </c>
+      <c r="N4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -5950,8 +7331,17 @@
       <c r="F5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>334</v>
+      </c>
+      <c r="L5" t="s">
+        <v>345</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -5970,8 +7360,17 @@
       <c r="F6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K6" t="s">
+        <v>334</v>
+      </c>
+      <c r="L6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -5993,8 +7392,14 @@
       <c r="G7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>334</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -6016,8 +7421,20 @@
       <c r="G8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>334</v>
+      </c>
+      <c r="L8" t="s">
+        <v>362</v>
+      </c>
+      <c r="N8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -6039,31 +7456,46 @@
       <c r="G9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="K9" t="s">
+        <v>335</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -6085,8 +7517,14 @@
       <c r="G11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>334</v>
+      </c>
+      <c r="L11" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -6105,8 +7543,14 @@
       <c r="F12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>334</v>
+      </c>
+      <c r="L12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -6125,28 +7569,40 @@
       <c r="F13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="K13" t="s">
+        <v>336</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -6168,8 +7624,17 @@
       <c r="G15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>334</v>
+      </c>
+      <c r="L15" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -6188,28 +7653,40 @@
       <c r="F16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="K16" t="s">
+        <v>334</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K17" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -6231,54 +7708,72 @@
       <c r="G18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="J18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" t="s">
+        <v>334</v>
+      </c>
+      <c r="L18" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="K19" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="B20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>107</v>
       </c>
@@ -6300,8 +7795,20 @@
       <c r="G21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" t="s">
+        <v>334</v>
+      </c>
+      <c r="L21" t="s">
+        <v>363</v>
+      </c>
+      <c r="N21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -6323,180 +7830,258 @@
       <c r="G22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" t="s">
+        <v>334</v>
+      </c>
+      <c r="L22" t="s">
+        <v>356</v>
+      </c>
+      <c r="N22" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="K23" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="B24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="K24" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="K25" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="K26" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="K27" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="K28" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="K29" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="B30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K30" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -6515,8 +8100,17 @@
       <c r="F31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>334</v>
+      </c>
+      <c r="L31" t="s">
+        <v>368</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>127</v>
       </c>
@@ -6535,28 +8129,43 @@
       <c r="F32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="K32" t="s">
+        <v>334</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="B33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K33" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>134</v>
       </c>
@@ -6575,36 +8184,54 @@
       <c r="F34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>334</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="K35" t="s">
+        <v>334</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="B36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -6623,31 +8250,44 @@
       <c r="F37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="K37" t="s">
+        <v>334</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -6666,8 +8306,14 @@
       <c r="F39" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>334</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -6689,33 +8335,51 @@
       <c r="G40" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>334</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="K41" t="s">
+        <v>334</v>
+      </c>
+      <c r="L41" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B42" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="B42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K42" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="M42" s="15" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -6734,31 +8398,46 @@
       <c r="F43" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="K43" t="s">
+        <v>334</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J44" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>161</v>
       </c>
@@ -6777,31 +8456,46 @@
       <c r="F45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="K45" t="s">
+        <v>334</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K46" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>163</v>
       </c>
@@ -6820,8 +8514,14 @@
       <c r="F47" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>334</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -6831,8 +8531,14 @@
       <c r="C48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>376</v>
+      </c>
+      <c r="K48" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>166</v>
       </c>
@@ -6851,8 +8557,14 @@
       <c r="F49" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>334</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>167</v>
       </c>
@@ -6874,8 +8586,14 @@
       <c r="G50" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>334</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -6894,8 +8612,14 @@
       <c r="F51" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>337</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -6914,74 +8638,101 @@
       <c r="F52" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="K52" t="s">
+        <v>334</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B53" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="B53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="K53" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B54" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="B54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="K54" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="B55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K55" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>177</v>
       </c>
@@ -7000,51 +8751,75 @@
       <c r="F56" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="K56" t="s">
+        <v>334</v>
+      </c>
+      <c r="M56" s="16" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="B57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="K57" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B58" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K58" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>181</v>
       </c>
@@ -7063,8 +8838,17 @@
       <c r="F59" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>334</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>186</v>
       </c>
@@ -7086,31 +8870,46 @@
       <c r="G60" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="K60" t="s">
+        <v>334</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B61" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="B61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K61" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>198</v>
       </c>
@@ -7132,8 +8931,17 @@
       <c r="G62" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K62" t="s">
+        <v>334</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>199</v>
       </c>
@@ -7152,8 +8960,11 @@
       <c r="F63" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K63" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>201</v>
       </c>
@@ -7175,24 +8986,36 @@
       <c r="G64" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
+        <v>33</v>
+      </c>
+      <c r="K65" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
@@ -7204,15 +9027,18 @@
         <v>11</v>
       </c>
       <c r="E66" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F66" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="K66" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
@@ -7224,15 +9050,21 @@
         <v>11</v>
       </c>
       <c r="E67" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="F67" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="G67" t="s">
+        <v>94</v>
+      </c>
+      <c r="K67" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
@@ -7252,24 +9084,39 @@
       <c r="G68" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E69" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69" t="s">
+        <v>18</v>
+      </c>
+      <c r="K69" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
@@ -7281,18 +9128,18 @@
         <v>11</v>
       </c>
       <c r="E70" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>93</v>
-      </c>
-      <c r="G70" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="K70" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -7312,24 +9159,36 @@
       <c r="G71" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K71" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="B72" t="s">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E72" t="s">
+        <v>43</v>
+      </c>
+      <c r="F72" t="s">
+        <v>44</v>
+      </c>
+      <c r="K72" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
@@ -7337,200 +9196,224 @@
       <c r="C73" t="s">
         <v>9</v>
       </c>
-      <c r="D73" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="K73" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>234</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="K74" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" t="s">
+        <v>17</v>
+      </c>
+      <c r="G75" t="s">
+        <v>18</v>
+      </c>
+      <c r="K75" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>239</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>11</v>
+      </c>
+      <c r="K76" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>240</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" t="s">
+        <v>26</v>
+      </c>
+      <c r="K77" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>249</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="K78" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>252</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" t="s">
+        <v>22</v>
+      </c>
+      <c r="F79" t="s">
+        <v>23</v>
+      </c>
+      <c r="K79" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>260</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="K80" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>264</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" t="s">
+        <v>33</v>
+      </c>
+      <c r="K81" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>271</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="K82" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>274</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" t="s">
         <v>43</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F83" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>230</v>
-      </c>
-      <c r="B74" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" t="s">
-        <v>16</v>
-      </c>
-      <c r="F74" t="s">
-        <v>17</v>
-      </c>
-      <c r="G74" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>231</v>
-      </c>
-      <c r="B75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" t="s">
-        <v>9</v>
-      </c>
-      <c r="D75" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" t="s">
-        <v>43</v>
-      </c>
-      <c r="F75" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>233</v>
-      </c>
-      <c r="B76" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>234</v>
-      </c>
-      <c r="B77" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>237</v>
-      </c>
-      <c r="B78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>9</v>
-      </c>
-      <c r="D78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" t="s">
-        <v>16</v>
-      </c>
-      <c r="F78" t="s">
-        <v>17</v>
-      </c>
-      <c r="G78" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>239</v>
-      </c>
-      <c r="B79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" t="s">
-        <v>9</v>
-      </c>
-      <c r="D79" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>240</v>
-      </c>
-      <c r="B80" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" t="s">
-        <v>9</v>
-      </c>
-      <c r="D80" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>249</v>
-      </c>
-      <c r="B81" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>252</v>
-      </c>
-      <c r="B82" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" t="s">
-        <v>9</v>
-      </c>
-      <c r="D82" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="K83" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>275</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
         <v>22</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F84" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>260</v>
-      </c>
-      <c r="B83" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>264</v>
-      </c>
-      <c r="B84" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" t="s">
-        <v>9</v>
-      </c>
-      <c r="D84" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" t="s">
-        <v>26</v>
-      </c>
-      <c r="F84" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K84" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
@@ -7538,10 +9421,16 @@
       <c r="C85" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>11</v>
+      </c>
+      <c r="K85" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>274</v>
+        <v>309</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
@@ -7558,10 +9447,13 @@
       <c r="F86" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K86" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>275</v>
+        <v>328</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
@@ -7573,15 +9465,21 @@
         <v>11</v>
       </c>
       <c r="E87" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F87" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="G87" t="s">
+        <v>330</v>
+      </c>
+      <c r="K87" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>277</v>
+        <v>331</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
@@ -7592,10 +9490,22 @@
       <c r="D88" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>26</v>
+      </c>
+      <c r="F88" t="s">
+        <v>27</v>
+      </c>
+      <c r="G88" t="s">
+        <v>183</v>
+      </c>
+      <c r="K88" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
@@ -7612,74 +9522,42 @@
       <c r="F89" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>328</v>
-      </c>
-      <c r="B90" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90" t="s">
-        <v>9</v>
-      </c>
-      <c r="D90" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" t="s">
-        <v>26</v>
-      </c>
-      <c r="F90" t="s">
-        <v>329</v>
-      </c>
-      <c r="G90" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>331</v>
-      </c>
-      <c r="B91" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" t="s">
-        <v>9</v>
-      </c>
-      <c r="D91" t="s">
-        <v>11</v>
-      </c>
-      <c r="E91" t="s">
-        <v>26</v>
-      </c>
-      <c r="F91" t="s">
-        <v>27</v>
-      </c>
-      <c r="G91" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>332</v>
-      </c>
-      <c r="B92" t="s">
-        <v>8</v>
-      </c>
-      <c r="C92" t="s">
-        <v>9</v>
-      </c>
-      <c r="D92" t="s">
-        <v>11</v>
-      </c>
-      <c r="E92" t="s">
-        <v>43</v>
-      </c>
-      <c r="F92" t="s">
-        <v>44</v>
+      <c r="K89" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F94" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F95" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F96" s="10" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="13" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>